<commit_message>
updating egret graphs and WQ graphs
</commit_message>
<xml_diff>
--- a/jumby_surveys/Egret_surveys.xlsx
+++ b/jumby_surveys/Egret_surveys.xlsx
@@ -282,10 +282,10 @@
     <t>Sponge</t>
   </si>
   <si>
-    <t>Gorgonian</t>
+    <t>Sponges &amp; soft coral</t>
   </si>
   <si>
-    <t>Soft coral</t>
+    <t>Gorgonian</t>
   </si>
   <si>
     <t>Porites porites</t>
@@ -3371,7 +3371,7 @@
       </c>
       <c r="H97" s="5" t="str">
         <f>VLOOKUP(E97,lookups!$2:$107,3,FALSE)</f>
-        <v>Soft coral</v>
+        <v>Sponges &amp; soft coral</v>
       </c>
     </row>
     <row r="98">
@@ -4351,7 +4351,7 @@
       </c>
       <c r="H132" s="5" t="str">
         <f>VLOOKUP(E132,lookups!$2:$107,3,FALSE)</f>
-        <v>Sponge</v>
+        <v>Sponges &amp; soft coral</v>
       </c>
     </row>
     <row r="133">
@@ -5154,8 +5154,8 @@
       <c r="E161" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F161" s="4">
-        <v>34.0</v>
+      <c r="F161" s="6">
+        <v>29.0</v>
       </c>
       <c r="G161" s="5" t="str">
         <f>VLOOKUP(E161,lookups!$2:$107,2,FALSE)</f>
@@ -9550,8 +9550,8 @@
       <c r="E318" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F318" s="4">
-        <v>48.0</v>
+      <c r="F318" s="6">
+        <v>38.0</v>
       </c>
       <c r="G318" s="5" t="str">
         <f>VLOOKUP(E318,lookups!$2:$107,2,FALSE)</f>
@@ -14954,8 +14954,8 @@
       <c r="E511" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F511" s="4">
-        <v>80.0</v>
+      <c r="F511" s="6">
+        <v>70.0</v>
       </c>
       <c r="G511" s="5" t="str">
         <f>VLOOKUP(E511,lookups!$2:$107,2,FALSE)</f>
@@ -17559,6 +17559,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="4" max="4" width="24.86"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -18136,8 +18139,8 @@
       <c r="B26" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>88</v>
+      <c r="C26" s="8" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="27">
@@ -18145,10 +18148,10 @@
         <v>27</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="28">

</xml_diff>